<commit_message>
Edit: Se actualizo el archivo con los link de las clases grabadas
</commit_message>
<xml_diff>
--- a/Links Clases Grabadas/ClasesGrabadas.xlsx
+++ b/Links Clases Grabadas/ClasesGrabadas.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mifvI3CWDAQWbY3SKCLZpT8Jrqt1Q=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjgkY1lo9bP5zvbp9DPHapFHCSz9w=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="73">
   <si>
     <t>Día</t>
   </si>
@@ -163,12 +163,50 @@
     <t>Asistir a clase habiendo leído la guía de Nexus</t>
   </si>
   <si>
-    <t>Guía de Nexus</t>
+    <r>
+      <rPr>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve">Guía de Nexus
+Clase grabada 4K3 año 2020 - Parte 1: </t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <sz val="11.0"/>
+        <u/>
+      </rPr>
+      <t>Nexus - Parte 1</t>
+    </r>
+  </si>
+  <si>
+    <t>Clase Grabada Nexus</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve">Clase grabada 4K3 año 2020 - Parte 2: </t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <sz val="11.0"/>
+        <u/>
+      </rPr>
+      <t>Nexus - Parte 2</t>
+    </r>
   </si>
   <si>
     <t>Práctico de Scrum - Planificación de release y sprint</t>
   </si>
   <si>
+    <t>Clase Grabada Practico 8</t>
+  </si>
+  <si>
     <t>Clase de Consulta</t>
   </si>
   <si>
@@ -179,6 +217,9 @@
   </si>
   <si>
     <t>Overview de Testing</t>
+  </si>
+  <si>
+    <t>Clase Grabada Testing</t>
   </si>
   <si>
     <t>Testing - Práctico de Caja Negra</t>
@@ -273,7 +314,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="12">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -303,6 +344,22 @@
       <u/>
       <sz val="11.0"/>
       <color theme="10"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11.0"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11.0"/>
+      <color rgb="FF1155CC"/>
+    </font>
+    <font/>
+    <font>
+      <u/>
+      <sz val="11.0"/>
+      <color rgb="FF1155CC"/>
     </font>
     <font>
       <b/>
@@ -343,7 +400,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border/>
     <border>
       <left style="thin">
@@ -369,11 +426,33 @@
       <top/>
       <bottom/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -397,6 +476,18 @@
     <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="1" fillId="3" fontId="2" numFmtId="16" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="16" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -406,12 +497,15 @@
     <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="16" xfId="0" applyFont="1" applyNumberFormat="1"/>
@@ -640,7 +734,7 @@
     <col customWidth="1" min="3" max="3" width="9.38"/>
     <col customWidth="1" min="4" max="4" width="41.38"/>
     <col customWidth="1" min="5" max="5" width="50.75"/>
-    <col customWidth="1" min="6" max="6" width="37.0"/>
+    <col customWidth="1" min="6" max="6" width="43.13"/>
     <col customWidth="1" min="7" max="7" width="42.0"/>
     <col customWidth="1" min="8" max="26" width="9.38"/>
   </cols>
@@ -715,7 +809,7 @@
         <v>14</v>
       </c>
       <c r="C4" s="4">
-        <f t="shared" ref="C4:C33" si="1">C2+7</f>
+        <f t="shared" ref="C4:C13" si="1">C2+7</f>
         <v>44278</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -898,232 +992,230 @@
       <c r="G12" s="7"/>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="12">
         <f t="shared" si="1"/>
         <v>44309</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="7"/>
+      <c r="G13" s="15" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="4">
-        <f t="shared" si="1"/>
-        <v>44313</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="7"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="16"/>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="4">
+        <f t="shared" ref="C15:C16" si="2">C12+7</f>
+        <v>44313</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="4">
-        <f t="shared" si="1"/>
+      <c r="C16" s="4">
+        <f t="shared" si="2"/>
         <v>44316</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="13">
-        <f t="shared" si="1"/>
-        <v>44320</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="15"/>
+      <c r="D16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>47</v>
+      </c>
       <c r="F16" s="3"/>
       <c r="G16" s="7"/>
     </row>
     <row r="17">
-      <c r="A17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="4">
-        <f t="shared" si="1"/>
-        <v>44323</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" s="3"/>
+      <c r="A17" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="19">
+        <f t="shared" ref="C17:C34" si="3">C15+7</f>
+        <v>44320</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="21"/>
       <c r="F17" s="3"/>
       <c r="G17" s="7"/>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C18" s="4">
-        <f t="shared" si="1"/>
-        <v>44327</v>
+        <f t="shared" si="3"/>
+        <v>44323</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F18" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G18" s="7"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="22" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C19" s="4">
-        <f t="shared" si="1"/>
-        <v>44330</v>
+        <f t="shared" si="3"/>
+        <v>44327</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="3"/>
+        <v>51</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="G19" s="7"/>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C20" s="4">
-        <f t="shared" si="1"/>
-        <v>44334</v>
+        <f t="shared" si="3"/>
+        <v>44330</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>52</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="E20" s="5"/>
       <c r="F20" s="3"/>
       <c r="G20" s="7"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21">
       <c r="A21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="4">
+        <f t="shared" si="3"/>
+        <v>44334</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="4">
-        <f t="shared" si="1"/>
+      <c r="C22" s="4">
+        <f t="shared" si="3"/>
         <v>44337</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="G21" s="7"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="8" t="s">
+      <c r="D22" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B23" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="9">
-        <f t="shared" si="1"/>
+      <c r="C23" s="9">
+        <f t="shared" si="3"/>
         <v>44341</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D23" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="7"/>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="4">
-        <f t="shared" si="1"/>
-        <v>44344</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="3"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="5"/>
       <c r="G23" s="7"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C24" s="4">
-        <f t="shared" si="1"/>
-        <v>44348</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>57</v>
+        <f t="shared" si="3"/>
+        <v>44344</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="3"/>
@@ -1131,178 +1223,195 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="4">
+        <f t="shared" si="3"/>
+        <v>44348</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B26" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="4">
-        <f t="shared" si="1"/>
+      <c r="C26" s="4">
+        <f t="shared" si="3"/>
         <v>44351</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F25" s="16"/>
-      <c r="G25" s="7"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="12" t="s">
+      <c r="D26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="23"/>
+      <c r="G26" s="7"/>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B27" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="13">
-        <f t="shared" si="1"/>
+      <c r="C27" s="19">
+        <f t="shared" si="3"/>
         <v>44355</v>
       </c>
-      <c r="D26" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="E26" s="15"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="7"/>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="4">
-        <f t="shared" si="1"/>
-        <v>44358</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>61</v>
-      </c>
+      <c r="D27" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="21"/>
       <c r="F27" s="3"/>
       <c r="G27" s="7"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C28" s="4">
-        <f t="shared" si="1"/>
-        <v>44362</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="E28" s="3"/>
+        <f t="shared" si="3"/>
+        <v>44358</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28" s="24" t="s">
+        <v>65</v>
+      </c>
       <c r="F28" s="3"/>
       <c r="G28" s="7"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C29" s="4">
-        <f t="shared" si="1"/>
-        <v>44365</v>
-      </c>
-      <c r="D29" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="E29" s="5"/>
+        <f t="shared" si="3"/>
+        <v>44362</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="7"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C30" s="4">
-        <f t="shared" si="1"/>
-        <v>44369</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F30" s="19" t="s">
-        <v>66</v>
-      </c>
+        <f t="shared" si="3"/>
+        <v>44365</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E30" s="5"/>
+      <c r="F30" s="3"/>
       <c r="G30" s="7"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="4">
+        <f t="shared" si="3"/>
+        <v>44369</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F31" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="G31" s="7"/>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B32" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="4">
-        <f t="shared" si="1"/>
+      <c r="C32" s="4">
+        <f t="shared" si="3"/>
         <v>44372</v>
       </c>
-      <c r="D31" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="E31" s="3"/>
-      <c r="G31" s="7"/>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="12" t="s">
+      <c r="D32" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" s="3"/>
+      <c r="G32" s="7"/>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B33" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="13">
-        <f t="shared" si="1"/>
+      <c r="C33" s="19">
+        <f t="shared" si="3"/>
         <v>44376</v>
       </c>
-      <c r="D32" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E32" s="15"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="7"/>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" s="4">
-        <f t="shared" si="1"/>
-        <v>44379</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E33" s="18"/>
+      <c r="D33" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E33" s="21"/>
       <c r="F33" s="3"/>
       <c r="G33" s="7"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="C34" s="20"/>
-      <c r="E34" s="21"/>
-    </row>
-    <row r="35" ht="15.75" customHeight="1"/>
+      <c r="A34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="4">
+        <f t="shared" si="3"/>
+        <v>44379</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E34" s="25"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="C35" s="27"/>
+      <c r="E35" s="28"/>
+    </row>
     <row r="36" ht="15.75" customHeight="1"/>
     <row r="37" ht="15.75" customHeight="1"/>
     <row r="38" ht="15.75" customHeight="1"/>
@@ -2268,7 +2377,16 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="G13:G14"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="G2"/>
     <hyperlink r:id="rId2" ref="G3"/>
@@ -2279,11 +2397,16 @@
     <hyperlink r:id="rId7" ref="G9"/>
     <hyperlink r:id="rId8" ref="G10"/>
     <hyperlink r:id="rId9" ref="G11"/>
-    <hyperlink r:id="rId10" ref="F30"/>
+    <hyperlink r:id="rId10" ref="F13"/>
+    <hyperlink r:id="rId11" ref="G13"/>
+    <hyperlink r:id="rId12" ref="F14"/>
+    <hyperlink r:id="rId13" ref="G15"/>
+    <hyperlink r:id="rId14" ref="G18"/>
+    <hyperlink r:id="rId15" ref="F31"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId11"/>
+  <drawing r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
edit: Se actualizo el doc del link de las clases grabadas
</commit_message>
<xml_diff>
--- a/Links Clases Grabadas/ClasesGrabadas.xlsx
+++ b/Links Clases Grabadas/ClasesGrabadas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="78">
   <si>
     <t>Día</t>
   </si>
@@ -229,19 +229,69 @@
 </t>
   </si>
   <si>
-    <t>Testing
-Parte 1: https://youtu.be/CkRfwRR5KJM
-Parte 2: https://youtu.be/MQPfWdtGYfw
-Parte 3: https://youtu.be/Oggb1RqDIaE</t>
+    <r>
+      <rPr>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve">Testing Caja Negra (Enlaces corregidos)
+Parte 1: </t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <sz val="11.0"/>
+        <u/>
+      </rPr>
+      <t xml:space="preserve"> Testing Caja Negra Parte 1
+</t>
+    </r>
+    <r>
+      <rPr>
+        <color theme="1"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t>Parte 2:</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF000000"/>
+        <sz val="11.0"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <sz val="11.0"/>
+        <u/>
+      </rPr>
+      <t>Testing Caja Negra Parte 2</t>
+    </r>
+  </si>
+  <si>
+    <t>Clase Grabada Testing Caja Negra</t>
   </si>
   <si>
     <t>Testing ágil en contexto</t>
   </si>
   <si>
+    <t>Clase Grabada Testing ágil</t>
+  </si>
+  <si>
     <t>Testing - Práctico de Caja Blanca</t>
   </si>
   <si>
     <t>Ver previamente video de Testing Caja Blanca</t>
+  </si>
+  <si>
+    <t>Testing Caja Blanca
+Parte 1: https://youtu.be/6IrH0k-2KQo
+Parte 2: https://youtu.be/Q7YP2x3DsSg
+Parte 3: https://youtu.be/wLFSbA537YI</t>
+  </si>
+  <si>
+    <t>Clase Grabada Testing Caja Blanca</t>
   </si>
   <si>
     <t>Filosofía Lean y Kanban</t>
@@ -252,6 +302,9 @@
   <si>
     <t>Aseguramiento de la calidad: https://youtu.be/GC0HejFmA5w
 CMMI y Auditorías lo ven por su cuenta: https://youtu.be/SUOfdl3Xew0</t>
+  </si>
+  <si>
+    <t>Clase Grabada Lean y Kanban</t>
   </si>
   <si>
     <t>Métricas tradicionales, Lean y Agile</t>
@@ -314,7 +367,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -337,10 +390,6 @@
       <color rgb="FF1155CC"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color theme="1"/>
-    </font>
-    <font>
       <u/>
       <sz val="11.0"/>
       <color theme="10"/>
@@ -360,6 +409,15 @@
       <u/>
       <sz val="11.0"/>
       <color rgb="FF1155CC"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11.0"/>
+      <color theme="1"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
     </font>
     <font>
       <b/>
@@ -452,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -470,24 +528,24 @@
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="1" fillId="3" fontId="2" numFmtId="16" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="16" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -497,15 +555,18 @@
     <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="11" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="16" xfId="0" applyFont="1" applyNumberFormat="1"/>
@@ -1120,10 +1181,12 @@
       <c r="E19" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="G19" s="7"/>
+      <c r="G19" s="6" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
@@ -1137,11 +1200,13 @@
         <v>44330</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="7"/>
+      <c r="G20" s="6" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
@@ -1155,13 +1220,17 @@
         <v>44334</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="7"/>
+        <v>58</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="3" t="s">
@@ -1175,15 +1244,17 @@
         <v>44337</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G22" s="7"/>
+        <v>63</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="8" t="s">
@@ -1215,7 +1286,7 @@
         <v>44344</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="3"/>
@@ -1233,7 +1304,7 @@
         <v>44348</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="3"/>
@@ -1254,9 +1325,9 @@
         <v>46</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="F26" s="23"/>
+        <v>67</v>
+      </c>
+      <c r="F26" s="25"/>
       <c r="G26" s="7"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
@@ -1271,7 +1342,7 @@
         <v>44355</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="E27" s="21"/>
       <c r="F27" s="3"/>
@@ -1289,10 +1360,10 @@
         <v>44358</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E28" s="24" t="s">
-        <v>65</v>
+        <v>69</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="7"/>
@@ -1308,8 +1379,8 @@
         <f t="shared" si="3"/>
         <v>44362</v>
       </c>
-      <c r="D29" s="24" t="s">
-        <v>66</v>
+      <c r="D29" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -1326,8 +1397,8 @@
         <f t="shared" si="3"/>
         <v>44365</v>
       </c>
-      <c r="D30" s="25" t="s">
-        <v>67</v>
+      <c r="D30" s="26" t="s">
+        <v>72</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="3"/>
@@ -1345,13 +1416,13 @@
         <v>44369</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F31" s="26" t="s">
-        <v>70</v>
+        <v>74</v>
+      </c>
+      <c r="F31" s="27" t="s">
+        <v>75</v>
       </c>
       <c r="G31" s="7"/>
     </row>
@@ -1366,8 +1437,8 @@
         <f t="shared" si="3"/>
         <v>44372</v>
       </c>
-      <c r="D32" s="25" t="s">
-        <v>67</v>
+      <c r="D32" s="26" t="s">
+        <v>72</v>
       </c>
       <c r="E32" s="3"/>
       <c r="G32" s="7"/>
@@ -1384,7 +1455,7 @@
         <v>44376</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="E33" s="21"/>
       <c r="F33" s="3"/>
@@ -1402,15 +1473,15 @@
         <v>44379</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E34" s="25"/>
+        <v>77</v>
+      </c>
+      <c r="E34" s="26"/>
       <c r="F34" s="3"/>
       <c r="G34" s="7"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="C35" s="27"/>
-      <c r="E35" s="28"/>
+      <c r="C35" s="28"/>
+      <c r="E35" s="29"/>
     </row>
     <row r="36" ht="15.75" customHeight="1"/>
     <row r="37" ht="15.75" customHeight="1"/>
@@ -2380,11 +2451,11 @@
     <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="D13:D14"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
     <mergeCell ref="G13:G14"/>
   </mergeCells>
   <hyperlinks>
@@ -2402,11 +2473,16 @@
     <hyperlink r:id="rId12" ref="F14"/>
     <hyperlink r:id="rId13" ref="G15"/>
     <hyperlink r:id="rId14" ref="G18"/>
-    <hyperlink r:id="rId15" ref="F31"/>
+    <hyperlink r:id="rId15" ref="F19"/>
+    <hyperlink r:id="rId16" ref="G19"/>
+    <hyperlink r:id="rId17" ref="G20"/>
+    <hyperlink r:id="rId18" ref="G21"/>
+    <hyperlink r:id="rId19" ref="G22"/>
+    <hyperlink r:id="rId20" ref="F31"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId16"/>
+  <drawing r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
edit: Se actualizo el archivo de clases grabadas
</commit_message>
<xml_diff>
--- a/Links Clases Grabadas/ClasesGrabadas.xlsx
+++ b/Links Clases Grabadas/ClasesGrabadas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="80">
   <si>
     <t>Día</t>
   </si>
@@ -310,7 +310,13 @@
     <t>Métricas tradicionales, Lean y Agile</t>
   </si>
   <si>
+    <t>Clase Grabada Métricas</t>
+  </si>
+  <si>
     <t>Ejecución de caja negra - Clase de Consulta práctico</t>
+  </si>
+  <si>
+    <t>Clase Grabada Repaso Caja Blanca + TP 12</t>
   </si>
   <si>
     <t>Fecha límite entrega Trabajo Conceptual 2</t>
@@ -367,7 +373,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -418,6 +424,11 @@
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11.0"/>
+      <color rgb="FF1155CC"/>
     </font>
     <font>
       <b/>
@@ -510,7 +521,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -564,9 +575,12 @@
     <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="11" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="12" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="16" xfId="0" applyFont="1" applyNumberFormat="1"/>
@@ -1289,7 +1303,9 @@
         <v>65</v>
       </c>
       <c r="E24" s="5"/>
-      <c r="F24" s="3"/>
+      <c r="F24" s="25" t="s">
+        <v>66</v>
+      </c>
       <c r="G24" s="7"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
@@ -1304,11 +1320,13 @@
         <v>44348</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="7"/>
+      <c r="G25" s="6" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="3" t="s">
@@ -1325,9 +1343,9 @@
         <v>46</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="F26" s="25"/>
+        <v>69</v>
+      </c>
+      <c r="F26" s="26"/>
       <c r="G26" s="7"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
@@ -1342,7 +1360,7 @@
         <v>44355</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E27" s="21"/>
       <c r="F27" s="3"/>
@@ -1360,10 +1378,10 @@
         <v>44358</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="7"/>
@@ -1380,7 +1398,7 @@
         <v>44362</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -1397,8 +1415,8 @@
         <f t="shared" si="3"/>
         <v>44365</v>
       </c>
-      <c r="D30" s="26" t="s">
-        <v>72</v>
+      <c r="D30" s="27" t="s">
+        <v>74</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="3"/>
@@ -1416,13 +1434,13 @@
         <v>44369</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F31" s="27" t="s">
-        <v>75</v>
+        <v>76</v>
+      </c>
+      <c r="F31" s="28" t="s">
+        <v>77</v>
       </c>
       <c r="G31" s="7"/>
     </row>
@@ -1437,8 +1455,8 @@
         <f t="shared" si="3"/>
         <v>44372</v>
       </c>
-      <c r="D32" s="26" t="s">
-        <v>72</v>
+      <c r="D32" s="27" t="s">
+        <v>74</v>
       </c>
       <c r="E32" s="3"/>
       <c r="G32" s="7"/>
@@ -1455,7 +1473,7 @@
         <v>44376</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E33" s="21"/>
       <c r="F33" s="3"/>
@@ -1473,15 +1491,15 @@
         <v>44379</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E34" s="26"/>
+        <v>79</v>
+      </c>
+      <c r="E34" s="27"/>
       <c r="F34" s="3"/>
       <c r="G34" s="7"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="C35" s="28"/>
-      <c r="E35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="E35" s="30"/>
     </row>
     <row r="36" ht="15.75" customHeight="1"/>
     <row r="37" ht="15.75" customHeight="1"/>
@@ -2478,11 +2496,13 @@
     <hyperlink r:id="rId17" ref="G20"/>
     <hyperlink r:id="rId18" ref="G21"/>
     <hyperlink r:id="rId19" ref="G22"/>
-    <hyperlink r:id="rId20" ref="F31"/>
+    <hyperlink r:id="rId20" ref="F24"/>
+    <hyperlink r:id="rId21" ref="G25"/>
+    <hyperlink r:id="rId22" ref="F31"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId21"/>
+  <drawing r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
edit: se actualizo archivo de clases grabadas
</commit_message>
<xml_diff>
--- a/Links Clases Grabadas/ClasesGrabadas.xlsx
+++ b/Links Clases Grabadas/ClasesGrabadas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="82">
   <si>
     <t>Día</t>
   </si>
@@ -325,13 +325,19 @@
     <t>Segundo Parcial</t>
   </si>
   <si>
-    <t>Comparación de enfoques tradicional, lean y agile</t>
-  </si>
-  <si>
-    <t>Deben traer para trabajar en clase un cuadro comparativo de los 3 enfoques (ver TP 14 en la guía de prácticos). Es evaluable</t>
+    <t>Retrospectiva</t>
+  </si>
+  <si>
+    <t>Deben traer para trabajar en clase un cuadro comparativo de los 3 enfoques (ver TP 14 en la guía de prácticos). Es evaluable. Se usará como recuperatorio de los TP conceptuales, para los grupos que lo necesiten</t>
+  </si>
+  <si>
+    <t>Clase Grabada Retrospectiva</t>
   </si>
   <si>
     <t>Publicidad en Instagram con herramientas de Design Thinking</t>
+  </si>
+  <si>
+    <t>Clase Grabada Practico 13</t>
   </si>
   <si>
     <t>Pecha Kucha</t>
@@ -521,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -579,6 +585,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="12" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -1366,7 +1375,7 @@
       <c r="F27" s="3"/>
       <c r="G27" s="7"/>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
+    <row r="28" ht="54.0" customHeight="1">
       <c r="A28" s="3" t="s">
         <v>11</v>
       </c>
@@ -1377,13 +1386,15 @@
         <f t="shared" si="3"/>
         <v>44358</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="F28" s="3"/>
+      <c r="F28" s="25" t="s">
+        <v>73</v>
+      </c>
       <c r="G28" s="7"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
@@ -1398,11 +1409,13 @@
         <v>44362</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="7"/>
+      <c r="G29" s="6" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="3" t="s">
@@ -1415,8 +1428,8 @@
         <f t="shared" si="3"/>
         <v>44365</v>
       </c>
-      <c r="D30" s="27" t="s">
-        <v>74</v>
+      <c r="D30" s="28" t="s">
+        <v>76</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="3"/>
@@ -1434,13 +1447,13 @@
         <v>44369</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F31" s="28" t="s">
-        <v>77</v>
+        <v>78</v>
+      </c>
+      <c r="F31" s="29" t="s">
+        <v>79</v>
       </c>
       <c r="G31" s="7"/>
     </row>
@@ -1455,8 +1468,8 @@
         <f t="shared" si="3"/>
         <v>44372</v>
       </c>
-      <c r="D32" s="27" t="s">
-        <v>74</v>
+      <c r="D32" s="28" t="s">
+        <v>76</v>
       </c>
       <c r="E32" s="3"/>
       <c r="G32" s="7"/>
@@ -1473,7 +1486,7 @@
         <v>44376</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E33" s="21"/>
       <c r="F33" s="3"/>
@@ -1491,15 +1504,15 @@
         <v>44379</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E34" s="27"/>
+        <v>81</v>
+      </c>
+      <c r="E34" s="28"/>
       <c r="F34" s="3"/>
       <c r="G34" s="7"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="C35" s="29"/>
-      <c r="E35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="E35" s="31"/>
     </row>
     <row r="36" ht="15.75" customHeight="1"/>
     <row r="37" ht="15.75" customHeight="1"/>
@@ -2498,11 +2511,13 @@
     <hyperlink r:id="rId19" ref="G22"/>
     <hyperlink r:id="rId20" ref="F24"/>
     <hyperlink r:id="rId21" ref="G25"/>
-    <hyperlink r:id="rId22" ref="F31"/>
+    <hyperlink r:id="rId22" ref="F28"/>
+    <hyperlink r:id="rId23" ref="G29"/>
+    <hyperlink r:id="rId24" ref="F31"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId23"/>
+  <drawing r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>